<commit_message>
Tweeking the numbers a bit
</commit_message>
<xml_diff>
--- a/Calculators/Spreadsheet Calculators/DGG-LossPotential.xlsx
+++ b/Calculators/Spreadsheet Calculators/DGG-LossPotential.xlsx
@@ -2468,9 +2468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>